<commit_message>
add account, key word sheet
</commit_message>
<xml_diff>
--- a/NodeCode.xlsx
+++ b/NodeCode.xlsx
@@ -1,36 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git\NoteCode\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F3D284-7A8B-4582-BD50-A9DE06694B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="10" r:id="rId1"/>
-    <sheet name="SQL" sheetId="11" r:id="rId2"/>
-    <sheet name="Error" sheetId="12" r:id="rId3"/>
-    <sheet name="abstrach_interface" sheetId="13" r:id="rId4"/>
+    <sheet name="KeyWord" sheetId="14" r:id="rId2"/>
+    <sheet name="SQL" sheetId="11" r:id="rId3"/>
+    <sheet name="Error" sheetId="12" r:id="rId4"/>
+    <sheet name="abstrach_interface" sheetId="13" r:id="rId5"/>
+    <sheet name="account" sheetId="15" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="254">
   <si>
     <t>Kiểm tra 1 số có phải là kiểu Double hay không?</t>
     <phoneticPr fontId="2"/>
@@ -907,11 +907,32 @@
   <si>
     <t>Đọc một dòng trong csv, nếu field có hoặc không có dấu ngoặc kép</t>
   </si>
+  <si>
+    <t>code thông minh</t>
+  </si>
+  <si>
+    <t>Code Playgrounds</t>
+  </si>
+  <si>
+    <t>intellisense</t>
+  </si>
+  <si>
+    <t>acer nitro 5</t>
+  </si>
+  <si>
+    <t>matuan</t>
+  </si>
+  <si>
+    <t>hin</t>
+  </si>
+  <si>
+    <t>pw</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -1080,11 +1101,11 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="4" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Excel Built-in Normal" xfId="2"/>
+    <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 2 2" xfId="4"/>
-    <cellStyle name="標準 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="標準 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1116,7 +1137,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="Group 3"/>
+        <xdr:cNvPr id="2" name="Group 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr>
           <a:grpSpLocks/>
         </xdr:cNvGrpSpPr>
@@ -1131,7 +1158,13 @@
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="3" name="Picture 1"/>
+          <xdr:cNvPr id="3" name="Picture 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -1184,7 +1217,13 @@
       </xdr:pic>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Rectangle 3"/>
+          <xdr:cNvPr id="4" name="Rectangle 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1244,7 +1283,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Down Arrow 4"/>
+        <xdr:cNvPr id="5" name="Down Arrow 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1297,7 +1342,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="6" name="Group 9"/>
+        <xdr:cNvPr id="6" name="Group 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr>
           <a:grpSpLocks/>
         </xdr:cNvGrpSpPr>
@@ -1312,7 +1363,13 @@
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="7" name="Picture 6"/>
+          <xdr:cNvPr id="7" name="Picture 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -1365,7 +1422,13 @@
       </xdr:pic>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="Rectangle 7"/>
+          <xdr:cNvPr id="8" name="Rectangle 7">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1409,7 +1472,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="9" name="Rectangular Callout 8"/>
+          <xdr:cNvPr id="9" name="Rectangular Callout 8">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1475,7 +1544,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="10" name="Group 24"/>
+        <xdr:cNvPr id="10" name="Group 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr>
           <a:grpSpLocks/>
         </xdr:cNvGrpSpPr>
@@ -1490,7 +1565,13 @@
       </xdr:grpSpPr>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="11" name="Group 22"/>
+          <xdr:cNvPr id="11" name="Group 22">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvGrpSpPr>
             <a:grpSpLocks/>
           </xdr:cNvGrpSpPr>
@@ -1505,7 +1586,13 @@
         </xdr:grpSpPr>
         <xdr:grpSp>
           <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="13" name="Group 17"/>
+            <xdr:cNvPr id="13" name="Group 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvGrpSpPr>
               <a:grpSpLocks/>
             </xdr:cNvGrpSpPr>
@@ -1520,7 +1607,13 @@
           </xdr:grpSpPr>
           <xdr:grpSp>
             <xdr:nvGrpSpPr>
-              <xdr:cNvPr id="16" name="Group 15"/>
+              <xdr:cNvPr id="16" name="Group 15">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
               <xdr:cNvGrpSpPr>
                 <a:grpSpLocks/>
               </xdr:cNvGrpSpPr>
@@ -1535,7 +1628,13 @@
             </xdr:grpSpPr>
             <xdr:pic>
               <xdr:nvPicPr>
-                <xdr:cNvPr id="18" name="Picture 11"/>
+                <xdr:cNvPr id="18" name="Picture 11">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
                 <xdr:cNvPicPr>
                   <a:picLocks noChangeAspect="1"/>
                 </xdr:cNvPicPr>
@@ -1588,7 +1687,13 @@
             </xdr:pic>
             <xdr:pic>
               <xdr:nvPicPr>
-                <xdr:cNvPr id="19" name="Picture 14"/>
+                <xdr:cNvPr id="19" name="Picture 14">
+                  <a:extLst>
+                    <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                      <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+                    </a:ext>
+                  </a:extLst>
+                </xdr:cNvPr>
                 <xdr:cNvPicPr>
                   <a:picLocks noChangeAspect="1"/>
                 </xdr:cNvPicPr>
@@ -1642,7 +1747,13 @@
           </xdr:grpSp>
           <xdr:pic>
             <xdr:nvPicPr>
-              <xdr:cNvPr id="17" name="Picture 16"/>
+              <xdr:cNvPr id="17" name="Picture 16">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
               <xdr:cNvPicPr>
                 <a:picLocks noChangeAspect="1"/>
               </xdr:cNvPicPr>
@@ -1696,7 +1807,13 @@
         </xdr:grpSp>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="Rectangle 13"/>
+            <xdr:cNvPr id="14" name="Rectangle 13">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -1740,7 +1857,13 @@
         </xdr:sp>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="15" name="Rectangle 14"/>
+            <xdr:cNvPr id="15" name="Rectangle 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
           <xdr:spPr>
@@ -1785,7 +1908,13 @@
       </xdr:grpSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="12" name="Rectangular Callout 11"/>
+          <xdr:cNvPr id="12" name="Rectangular Callout 11">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -1851,7 +1980,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="20" name="Group 32"/>
+        <xdr:cNvPr id="20" name="Group 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr>
           <a:grpSpLocks/>
         </xdr:cNvGrpSpPr>
@@ -1866,7 +2001,13 @@
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="21" name="Picture 29"/>
+          <xdr:cNvPr id="21" name="Picture 29">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -1919,7 +2060,13 @@
       </xdr:pic>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="22" name="Picture 30"/>
+          <xdr:cNvPr id="22" name="Picture 30">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -1972,7 +2119,13 @@
       </xdr:pic>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="23" name="Rectangle 22"/>
+          <xdr:cNvPr id="23" name="Rectangle 22">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2032,7 +2185,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="24" name="Group 25"/>
+        <xdr:cNvPr id="24" name="Group 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr>
           <a:grpSpLocks/>
         </xdr:cNvGrpSpPr>
@@ -2047,7 +2206,13 @@
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="25" name="Picture 23"/>
+          <xdr:cNvPr id="25" name="Picture 23">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -2100,7 +2265,13 @@
       </xdr:pic>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="26" name="Rectangular Callout 25"/>
+          <xdr:cNvPr id="26" name="Rectangular Callout 25">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2166,7 +2337,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="27" name="Group 28"/>
+        <xdr:cNvPr id="27" name="Group 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr>
           <a:grpSpLocks/>
         </xdr:cNvGrpSpPr>
@@ -2181,7 +2358,13 @@
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="28" name="Picture 26"/>
+          <xdr:cNvPr id="28" name="Picture 26">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -2234,7 +2417,13 @@
       </xdr:pic>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="29" name="Rectangle 28"/>
+          <xdr:cNvPr id="29" name="Rectangle 28">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2294,7 +2483,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="30" name="Group 31"/>
+        <xdr:cNvPr id="30" name="Group 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr>
           <a:grpSpLocks/>
         </xdr:cNvGrpSpPr>
@@ -2309,7 +2504,13 @@
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="31" name="Picture 29"/>
+          <xdr:cNvPr id="31" name="Picture 29">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001F000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -2362,7 +2563,13 @@
       </xdr:pic>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="32" name="Rectangle 31"/>
+          <xdr:cNvPr id="32" name="Rectangle 31">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2422,7 +2629,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="33" name="Group 35"/>
+        <xdr:cNvPr id="33" name="Group 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr>
           <a:grpSpLocks/>
         </xdr:cNvGrpSpPr>
@@ -2437,7 +2650,13 @@
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="34" name="Picture 32"/>
+          <xdr:cNvPr id="34" name="Picture 32">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvPicPr>
             <a:picLocks noChangeAspect="1"/>
           </xdr:cNvPicPr>
@@ -2490,7 +2709,13 @@
       </xdr:pic>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="35" name="Rectangle 34"/>
+          <xdr:cNvPr id="35" name="Rectangle 34">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2534,7 +2759,13 @@
       </xdr:sp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="36" name="Rectangle 35"/>
+          <xdr:cNvPr id="36" name="Rectangle 35">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
@@ -2594,7 +2825,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="Picture 36"/>
+        <xdr:cNvPr id="37" name="Picture 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2662,7 +2899,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="Picture 37"/>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2730,7 +2973,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="39" name="Picture 38"/>
+        <xdr:cNvPr id="39" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000027000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2798,7 +3047,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="40" name="Picture 39"/>
+        <xdr:cNvPr id="40" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2866,7 +3121,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="41" name="Picture 1"/>
+        <xdr:cNvPr id="41" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000029000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3177,17 +3438,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G479"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -3770,7 +4031,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0B24AD-9310-4007-8959-7F533288A05D}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:B85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4171,8 +4461,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4222,8 +4512,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:B194"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4991,6 +5281,48 @@
     <row r="194" spans="2:2">
       <c r="B194" s="7" t="s">
         <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C56CCA-2F09-44DE-ABDB-9B2FE9502CF2}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4">
+        <v>14111996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add fulltext tutorial, text link
</commit_message>
<xml_diff>
--- a/NodeCode.xlsx
+++ b/NodeCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git\NoteCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F3D284-7A8B-4582-BD50-A9DE06694B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D9CF50-BD8C-454F-B0CA-D7042C8ED564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="10" r:id="rId1"/>
@@ -3448,7 +3448,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G479"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A460" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A481" sqref="A481"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -5292,7 +5294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C56CCA-2F09-44DE-ABDB-9B2FE9502CF2}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>

</xml_diff>

<commit_message>
no update, test git
</commit_message>
<xml_diff>
--- a/NodeCode.xlsx
+++ b/NodeCode.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git\NoteCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D9CF50-BD8C-454F-B0CA-D7042C8ED564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="10" r:id="rId1"/>
@@ -932,19 +931,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -953,7 +952,7 @@
       <u/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="major"/>
@@ -974,7 +973,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -983,7 +982,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1013,7 +1012,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1035,7 +1034,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1101,11 +1100,11 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="4" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="標準 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2 2" xfId="4"/>
+    <cellStyle name="標準 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1150,8 +1149,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="605118" y="1165412"/>
-          <a:ext cx="7866529" cy="466725"/>
+          <a:off x="683559" y="1053353"/>
+          <a:ext cx="8886265" cy="421901"/>
           <a:chOff x="685800" y="1066800"/>
           <a:chExt cx="8904763" cy="428625"/>
         </a:xfrm>
@@ -1355,8 +1354,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="605118" y="2308412"/>
-          <a:ext cx="8519272" cy="6981825"/>
+          <a:off x="683559" y="2061882"/>
+          <a:ext cx="9617448" cy="6175002"/>
           <a:chOff x="685800" y="2095500"/>
           <a:chExt cx="9647620" cy="6295239"/>
         </a:xfrm>
@@ -1557,8 +1556,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="605118" y="9928412"/>
-          <a:ext cx="8919322" cy="20716875"/>
+          <a:off x="683559" y="8785412"/>
+          <a:ext cx="10017498" cy="18296404"/>
           <a:chOff x="676275" y="8953500"/>
           <a:chExt cx="10057144" cy="18659320"/>
         </a:xfrm>
@@ -1993,8 +1992,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9681882" y="9928412"/>
-          <a:ext cx="6903944" cy="10363200"/>
+          <a:off x="10936941" y="8785412"/>
+          <a:ext cx="7766797" cy="9152964"/>
           <a:chOff x="10972800" y="8953500"/>
           <a:chExt cx="7790477" cy="9334069"/>
         </a:xfrm>
@@ -2198,8 +2197,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="605118" y="31264412"/>
-          <a:ext cx="6894419" cy="5762625"/>
+          <a:off x="683559" y="27611294"/>
+          <a:ext cx="7757272" cy="5090272"/>
           <a:chOff x="683559" y="27611294"/>
           <a:chExt cx="7761905" cy="5085715"/>
         </a:xfrm>
@@ -2350,8 +2349,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="605118" y="37741412"/>
-          <a:ext cx="8057029" cy="6600825"/>
+          <a:off x="683559" y="33326294"/>
+          <a:ext cx="9076765" cy="5838825"/>
           <a:chOff x="683559" y="33326294"/>
           <a:chExt cx="9076191" cy="5838096"/>
         </a:xfrm>
@@ -2496,8 +2495,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9076765" y="38884412"/>
-          <a:ext cx="5098116" cy="4143375"/>
+          <a:off x="10253382" y="34334824"/>
+          <a:ext cx="5725646" cy="3672727"/>
           <a:chOff x="10253382" y="34334824"/>
           <a:chExt cx="5723810" cy="3676191"/>
         </a:xfrm>
@@ -2642,8 +2641,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="605118" y="44980412"/>
-          <a:ext cx="6780119" cy="6562725"/>
+          <a:off x="683559" y="39713647"/>
+          <a:ext cx="7642972" cy="5800725"/>
           <a:chOff x="683559" y="39377471"/>
           <a:chExt cx="7647620" cy="5800000"/>
         </a:xfrm>
@@ -3445,14 +3444,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G479"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A460" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A451" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A481" sqref="A481"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="16384" width="9" style="2"/>
@@ -4026,6 +4025,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -4033,12 +4033,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0B24AD-9310-4007-8959-7F533288A05D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4056,21 +4056,22 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6"/>
-    <col min="2" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="9.125" style="6"/>
+    <col min="2" max="16384" width="9.125" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2">
@@ -4459,19 +4460,20 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="16384" width="9.125" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2">
@@ -4484,45 +4486,46 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" ht="14.25">
       <c r="B4" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="2:2" ht="15">
       <c r="B5" s="10" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:2" ht="15">
       <c r="B6" s="10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="2:2" ht="15">
       <c r="B7" s="10" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="2:2">
+    <row r="8" spans="2:2" ht="14.25">
       <c r="B8" s="10" t="s">
         <v>136</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B194"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="16384" width="9.125" style="7"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2">
@@ -5286,17 +5289,18 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C56CCA-2F09-44DE-ABDB-9B2FE9502CF2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -5328,6 +5332,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>